<commit_message>
added new 70 malicious xlsx
</commit_message>
<xml_diff>
--- a/CrowdsourcingReliableRatings/Charts.xlsx
+++ b/CrowdsourcingReliableRatings/Charts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\psko\Desktop\phd\DriverSense\CrowdsourcingReliableRatings\CrowdsourcingReliableRatings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2617F22-D52C-489C-9E74-CE5A28C7B28D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534C2DF1-F2FF-4A79-9C27-5E03883B166E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="2670" windowWidth="29040" windowHeight="16440" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Total Amount for each rating" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Chart average rating per Worker" sheetId="2" r:id="rId4"/>
     <sheet name="Chart RMSE sample size" sheetId="3" r:id="rId5"/>
     <sheet name="Chart Varying population" sheetId="4" r:id="rId6"/>
+    <sheet name="Chart 70 Malicious" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="161">
   <si>
     <t>Ratings</t>
   </si>
@@ -480,6 +481,39 @@
   </si>
   <si>
     <t>RMSE(Recommended)</t>
+  </si>
+  <si>
+    <t>RMSE Random</t>
+  </si>
+  <si>
+    <t>RMSE Average</t>
+  </si>
+  <si>
+    <t>RMSE Recommended</t>
+  </si>
+  <si>
+    <t>Malicious(0)</t>
+  </si>
+  <si>
+    <t>Malicious(10)</t>
+  </si>
+  <si>
+    <t>Malicious(20)</t>
+  </si>
+  <si>
+    <t>Malicious(30)</t>
+  </si>
+  <si>
+    <t>Malicious(40)</t>
+  </si>
+  <si>
+    <t>Malicious(50)</t>
+  </si>
+  <si>
+    <t>Malicious(60)</t>
+  </si>
+  <si>
+    <t>Malicious(70)</t>
   </si>
 </sst>
 </file>
@@ -3789,7 +3823,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -6208,6 +6241,1201 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="414431976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Chart 70 Malicious'!$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Malicious(0)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Chart 70 Malicious'!$A$20:$A$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart 70 Malicious'!$B$20:$B$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.2108511535458267</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21085115354582662</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.21085115354582673</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16966621725300246</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.13859000277215855</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.12220452672241615</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.1160529221268705</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.12143541558475808</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.12846635250062063</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.13499768768818382</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-50D7-41C1-808E-EC9EC379EB96}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Chart 70 Malicious'!$C$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Malicious(10)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Chart 70 Malicious'!$A$20:$A$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart 70 Malicious'!$C$20:$C$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.190878978</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.190878978</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.190878978</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15486550099999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.13111799399999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.118521707</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.11202870400000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.118670527</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.131595405</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.14324272699999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-50D7-41C1-808E-EC9EC379EB96}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Chart 70 Malicious'!$D$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Malicious(20)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Chart 70 Malicious'!$A$20:$A$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart 70 Malicious'!$D$20:$D$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.179495399</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.179495399</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.179495399</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.14511374599999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.12653077700000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11970107100000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.116201965</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.123657663</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.134050956</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.14312531100000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-50D7-41C1-808E-EC9EC379EB96}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Chart 70 Malicious'!$E$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Malicious(30)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Chart 70 Malicious'!$A$20:$A$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart 70 Malicious'!$E$20:$E$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.17321540099999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.17321540099999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.17321540099999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.14105674900000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.12363901400000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.12211119500000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.12841448899999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.13525158700000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.139147679</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.149502937</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-50D7-41C1-808E-EC9EC379EB96}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Chart 70 Malicious'!$F$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Malicious(40)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Chart 70 Malicious'!$A$20:$A$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart 70 Malicious'!$F$20:$F$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.151891045</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.15819113400000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.16161914199999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.14404299200000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.13298987600000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.12891243999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.131943372</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.13947631699999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.14704895100000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.152172115</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-50D7-41C1-808E-EC9EC379EB96}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Chart 70 Malicious'!$G$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Malicious(50)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Chart 70 Malicious'!$A$20:$A$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart 70 Malicious'!$G$20:$G$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.17253289599999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.17253289599999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.17253289599999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16570743099999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.171088501</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.177861084</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.18955254899999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.22140120199999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.25998965800000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.28433275800000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-50D7-41C1-808E-EC9EC379EB96}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Chart 70 Malicious'!$H$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Malicious(60)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Chart 70 Malicious'!$A$20:$A$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart 70 Malicious'!$H$20:$H$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.60561447899999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.606660541</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.60649472999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.60630627199999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.60601994100000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.60595386299999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.60591082500000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.60483277800000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.60450866599999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.60466670499999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-50D7-41C1-808E-EC9EC379EB96}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Chart 70 Malicious'!$I$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Malicious(70)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Chart 70 Malicious'!$A$20:$A$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chart 70 Malicious'!$I$20:$I$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.57044078099999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.56909805000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.56874962299999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.56795775599999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.56783326300000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.56741669100000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.56692750400000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.56571251899999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.56596915699999994</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.56607788199999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-50D7-41C1-808E-EC9EC379EB96}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="570922392"/>
+        <c:axId val="570922064"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="570922392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Sample Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="570922064"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="570922064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>RMSE</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="570922392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6607,6 +7835,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="341">
   <cs:axisTitle>
@@ -10167,6 +11435,509 @@
 </file>
 
 <file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -10987,6 +12758,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1250495</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>151039</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>489857</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA2C0BC6-F733-46C9-A994-2AE1D46A3A54}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -12993,7 +14805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B37CC8C6-B13E-4209-A526-16597264701D}">
   <dimension ref="A1:B71"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
@@ -13581,7 +15393,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:K1"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13989,7 +15801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9254DDDE-C450-4E55-8C17-34D685649580}">
   <dimension ref="A2:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
@@ -14176,4 +15988,1957 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F0F2733-BA40-47D7-8D0D-F4A0A3A7DE07}">
+  <dimension ref="A1:AU33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>70</v>
+      </c>
+      <c r="G1">
+        <v>80</v>
+      </c>
+      <c r="M1">
+        <v>90</v>
+      </c>
+      <c r="S1">
+        <v>100</v>
+      </c>
+      <c r="Y1">
+        <v>110</v>
+      </c>
+      <c r="AE1">
+        <v>120</v>
+      </c>
+      <c r="AL1">
+        <v>130</v>
+      </c>
+      <c r="AR1">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>150</v>
+      </c>
+      <c r="I2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J2" t="s">
+        <v>152</v>
+      </c>
+      <c r="M2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" t="s">
+        <v>150</v>
+      </c>
+      <c r="O2" t="s">
+        <v>151</v>
+      </c>
+      <c r="P2" t="s">
+        <v>152</v>
+      </c>
+      <c r="S2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T2" t="s">
+        <v>150</v>
+      </c>
+      <c r="U2" t="s">
+        <v>151</v>
+      </c>
+      <c r="V2" t="s">
+        <v>152</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>150</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>152</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>150</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>151</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>152</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>150</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>152</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>150</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>0.23646410975238807</v>
+      </c>
+      <c r="C3">
+        <v>0.71709620241127892</v>
+      </c>
+      <c r="D3">
+        <v>0.2108511535458267</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>0.33301061599999998</v>
+      </c>
+      <c r="I3">
+        <v>0.71944465800000001</v>
+      </c>
+      <c r="J3">
+        <v>0.190878978</v>
+      </c>
+      <c r="M3">
+        <v>5</v>
+      </c>
+      <c r="N3">
+        <v>0.33063724500000002</v>
+      </c>
+      <c r="O3">
+        <v>0.742274086</v>
+      </c>
+      <c r="P3">
+        <v>0.179495399</v>
+      </c>
+      <c r="S3">
+        <v>5</v>
+      </c>
+      <c r="T3">
+        <v>0.48385525600000001</v>
+      </c>
+      <c r="U3">
+        <v>0.76848581900000001</v>
+      </c>
+      <c r="V3">
+        <v>0.17321540099999999</v>
+      </c>
+      <c r="Y3">
+        <v>5</v>
+      </c>
+      <c r="Z3">
+        <v>0.63645217799999998</v>
+      </c>
+      <c r="AA3">
+        <v>0.58054052199999995</v>
+      </c>
+      <c r="AB3">
+        <v>0.151891045</v>
+      </c>
+      <c r="AE3">
+        <v>5</v>
+      </c>
+      <c r="AF3">
+        <v>0.45654898300000002</v>
+      </c>
+      <c r="AG3">
+        <v>0.82508193900000004</v>
+      </c>
+      <c r="AH3">
+        <v>0.17253289599999999</v>
+      </c>
+      <c r="AL3">
+        <v>5</v>
+      </c>
+      <c r="AM3">
+        <v>0.55541735199999998</v>
+      </c>
+      <c r="AN3">
+        <v>0.88976508600000004</v>
+      </c>
+      <c r="AO3">
+        <v>0.60561447899999998</v>
+      </c>
+      <c r="AR3">
+        <v>5</v>
+      </c>
+      <c r="AS3">
+        <v>0.63736985899999998</v>
+      </c>
+      <c r="AT3">
+        <v>1.0215142779999999</v>
+      </c>
+      <c r="AU3">
+        <v>0.57044078099999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>0.38674705410513216</v>
+      </c>
+      <c r="C4">
+        <v>0.71709620241127892</v>
+      </c>
+      <c r="D4">
+        <v>0.21085115354582662</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>0.20358121800000001</v>
+      </c>
+      <c r="I4">
+        <v>0.71944465800000001</v>
+      </c>
+      <c r="J4">
+        <v>0.190878978</v>
+      </c>
+      <c r="M4">
+        <v>10</v>
+      </c>
+      <c r="N4">
+        <v>0.24466243700000001</v>
+      </c>
+      <c r="O4">
+        <v>0.742274086</v>
+      </c>
+      <c r="P4">
+        <v>0.179495399</v>
+      </c>
+      <c r="S4">
+        <v>10</v>
+      </c>
+      <c r="T4">
+        <v>0.28976610200000003</v>
+      </c>
+      <c r="U4">
+        <v>0.76848581900000001</v>
+      </c>
+      <c r="V4">
+        <v>0.17321540099999999</v>
+      </c>
+      <c r="Y4">
+        <v>10</v>
+      </c>
+      <c r="Z4">
+        <v>0.45777160900000002</v>
+      </c>
+      <c r="AA4">
+        <v>0.68152702700000001</v>
+      </c>
+      <c r="AB4">
+        <v>0.15819113400000001</v>
+      </c>
+      <c r="AE4">
+        <v>10</v>
+      </c>
+      <c r="AF4">
+        <v>0.33326151399999998</v>
+      </c>
+      <c r="AG4">
+        <v>0.82508193900000004</v>
+      </c>
+      <c r="AH4">
+        <v>0.17253289599999999</v>
+      </c>
+      <c r="AL4">
+        <v>10</v>
+      </c>
+      <c r="AM4">
+        <v>0.32137901600000002</v>
+      </c>
+      <c r="AN4">
+        <v>0.78239149600000002</v>
+      </c>
+      <c r="AO4">
+        <v>0.606660541</v>
+      </c>
+      <c r="AR4">
+        <v>10</v>
+      </c>
+      <c r="AS4">
+        <v>0.29667360700000001</v>
+      </c>
+      <c r="AT4">
+        <v>0.79815538900000005</v>
+      </c>
+      <c r="AU4">
+        <v>0.56909805000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>0.19057627240826674</v>
+      </c>
+      <c r="C5">
+        <v>0.71709620241127892</v>
+      </c>
+      <c r="D5">
+        <v>0.21085115354582673</v>
+      </c>
+      <c r="G5">
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <v>0.36627565400000001</v>
+      </c>
+      <c r="I5">
+        <v>0.71944465800000001</v>
+      </c>
+      <c r="J5">
+        <v>0.190878978</v>
+      </c>
+      <c r="M5">
+        <v>15</v>
+      </c>
+      <c r="N5">
+        <v>0.24961249399999999</v>
+      </c>
+      <c r="O5">
+        <v>0.742274086</v>
+      </c>
+      <c r="P5">
+        <v>0.179495399</v>
+      </c>
+      <c r="S5">
+        <v>15</v>
+      </c>
+      <c r="T5">
+        <v>0.21738749600000001</v>
+      </c>
+      <c r="U5">
+        <v>0.76848581900000001</v>
+      </c>
+      <c r="V5">
+        <v>0.17321540099999999</v>
+      </c>
+      <c r="Y5">
+        <v>15</v>
+      </c>
+      <c r="Z5">
+        <v>0.22064281399999999</v>
+      </c>
+      <c r="AA5">
+        <v>0.71850953200000001</v>
+      </c>
+      <c r="AB5">
+        <v>0.16161914199999999</v>
+      </c>
+      <c r="AE5">
+        <v>15</v>
+      </c>
+      <c r="AF5">
+        <v>0.21595283500000001</v>
+      </c>
+      <c r="AG5">
+        <v>0.82508193900000004</v>
+      </c>
+      <c r="AH5">
+        <v>0.17253289599999999</v>
+      </c>
+      <c r="AL5">
+        <v>15</v>
+      </c>
+      <c r="AM5">
+        <v>0.22288392900000001</v>
+      </c>
+      <c r="AN5">
+        <v>0.72216792200000002</v>
+      </c>
+      <c r="AO5">
+        <v>0.60649472999999998</v>
+      </c>
+      <c r="AR5">
+        <v>15</v>
+      </c>
+      <c r="AS5">
+        <v>0.31860586499999999</v>
+      </c>
+      <c r="AT5">
+        <v>0.72845638599999996</v>
+      </c>
+      <c r="AU5">
+        <v>0.56874962299999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>0.18133468102649544</v>
+      </c>
+      <c r="C6">
+        <v>0.48152638157568317</v>
+      </c>
+      <c r="D6">
+        <v>0.16966621725300246</v>
+      </c>
+      <c r="G6">
+        <v>20</v>
+      </c>
+      <c r="H6">
+        <v>0.20351143299999999</v>
+      </c>
+      <c r="I6">
+        <v>0.46919928</v>
+      </c>
+      <c r="J6">
+        <v>0.15486550099999999</v>
+      </c>
+      <c r="M6">
+        <v>20</v>
+      </c>
+      <c r="N6">
+        <v>0.22719344899999999</v>
+      </c>
+      <c r="O6">
+        <v>0.50339824399999999</v>
+      </c>
+      <c r="P6">
+        <v>0.14511374599999999</v>
+      </c>
+      <c r="S6">
+        <v>20</v>
+      </c>
+      <c r="T6">
+        <v>0.214039433</v>
+      </c>
+      <c r="U6">
+        <v>0.54300161800000002</v>
+      </c>
+      <c r="V6">
+        <v>0.14105674900000001</v>
+      </c>
+      <c r="Y6">
+        <v>20</v>
+      </c>
+      <c r="Z6">
+        <v>0.186106875</v>
+      </c>
+      <c r="AA6">
+        <v>0.58858145100000003</v>
+      </c>
+      <c r="AB6">
+        <v>0.14404299200000001</v>
+      </c>
+      <c r="AE6">
+        <v>20</v>
+      </c>
+      <c r="AF6">
+        <v>0.29467514099999997</v>
+      </c>
+      <c r="AG6">
+        <v>0.70351487999999995</v>
+      </c>
+      <c r="AH6">
+        <v>0.16570743099999999</v>
+      </c>
+      <c r="AL6">
+        <v>20</v>
+      </c>
+      <c r="AM6">
+        <v>0.30730581099999998</v>
+      </c>
+      <c r="AN6">
+        <v>0.68064040400000003</v>
+      </c>
+      <c r="AO6">
+        <v>0.60630627199999998</v>
+      </c>
+      <c r="AR6">
+        <v>20</v>
+      </c>
+      <c r="AS6">
+        <v>0.26625422300000001</v>
+      </c>
+      <c r="AT6">
+        <v>0.65109263100000003</v>
+      </c>
+      <c r="AU6">
+        <v>0.56795775599999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>0.15561118950948402</v>
+      </c>
+      <c r="C7">
+        <v>0.27041437315654565</v>
+      </c>
+      <c r="D7">
+        <v>0.13859000277215855</v>
+      </c>
+      <c r="G7">
+        <v>25</v>
+      </c>
+      <c r="H7">
+        <v>0.150314853</v>
+      </c>
+      <c r="I7">
+        <v>0.29137450199999998</v>
+      </c>
+      <c r="J7">
+        <v>0.13111799399999999</v>
+      </c>
+      <c r="M7">
+        <v>25</v>
+      </c>
+      <c r="N7">
+        <v>0.21033189499999999</v>
+      </c>
+      <c r="O7">
+        <v>0.35126291300000001</v>
+      </c>
+      <c r="P7">
+        <v>0.12653077700000001</v>
+      </c>
+      <c r="S7">
+        <v>25</v>
+      </c>
+      <c r="T7">
+        <v>0.18547441200000001</v>
+      </c>
+      <c r="U7">
+        <v>0.41110438799999999</v>
+      </c>
+      <c r="V7">
+        <v>0.12363901400000001</v>
+      </c>
+      <c r="Y7">
+        <v>25</v>
+      </c>
+      <c r="Z7">
+        <v>0.16956685299999999</v>
+      </c>
+      <c r="AA7">
+        <v>0.48980715000000002</v>
+      </c>
+      <c r="AB7">
+        <v>0.13298987600000001</v>
+      </c>
+      <c r="AE7">
+        <v>25</v>
+      </c>
+      <c r="AF7">
+        <v>0.26489869300000002</v>
+      </c>
+      <c r="AG7">
+        <v>0.64221098799999998</v>
+      </c>
+      <c r="AH7">
+        <v>0.171088501</v>
+      </c>
+      <c r="AL7">
+        <v>25</v>
+      </c>
+      <c r="AM7">
+        <v>0.19522468400000001</v>
+      </c>
+      <c r="AN7">
+        <v>0.65795603999999996</v>
+      </c>
+      <c r="AO7">
+        <v>0.60601994100000001</v>
+      </c>
+      <c r="AR7">
+        <v>25</v>
+      </c>
+      <c r="AS7">
+        <v>0.17308404299999999</v>
+      </c>
+      <c r="AT7">
+        <v>0.63716946399999996</v>
+      </c>
+      <c r="AU7">
+        <v>0.56783326300000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>30</v>
+      </c>
+      <c r="B8">
+        <v>8.6213871961222099E-2</v>
+      </c>
+      <c r="C8">
+        <v>0.14021363680319482</v>
+      </c>
+      <c r="D8">
+        <v>0.12220452672241615</v>
+      </c>
+      <c r="G8">
+        <v>30</v>
+      </c>
+      <c r="H8">
+        <v>0.13844230599999999</v>
+      </c>
+      <c r="I8">
+        <v>0.20810498799999999</v>
+      </c>
+      <c r="J8">
+        <v>0.118521707</v>
+      </c>
+      <c r="M8">
+        <v>30</v>
+      </c>
+      <c r="N8">
+        <v>0.13319647900000001</v>
+      </c>
+      <c r="O8">
+        <v>0.29445397400000001</v>
+      </c>
+      <c r="P8">
+        <v>0.11970107100000001</v>
+      </c>
+      <c r="S8">
+        <v>30</v>
+      </c>
+      <c r="T8">
+        <v>0.144988389</v>
+      </c>
+      <c r="U8">
+        <v>0.37283121400000002</v>
+      </c>
+      <c r="V8">
+        <v>0.12211119500000001</v>
+      </c>
+      <c r="Y8">
+        <v>30</v>
+      </c>
+      <c r="Z8">
+        <v>0.17410462900000001</v>
+      </c>
+      <c r="AA8">
+        <v>0.43126250999999999</v>
+      </c>
+      <c r="AB8">
+        <v>0.12891243999999999</v>
+      </c>
+      <c r="AE8">
+        <v>30</v>
+      </c>
+      <c r="AF8">
+        <v>0.17891396300000001</v>
+      </c>
+      <c r="AG8">
+        <v>0.56899264500000002</v>
+      </c>
+      <c r="AH8">
+        <v>0.177861084</v>
+      </c>
+      <c r="AL8">
+        <v>30</v>
+      </c>
+      <c r="AM8">
+        <v>0.153849715</v>
+      </c>
+      <c r="AN8">
+        <v>0.64628294799999997</v>
+      </c>
+      <c r="AO8">
+        <v>0.60595386299999998</v>
+      </c>
+      <c r="AR8">
+        <v>30</v>
+      </c>
+      <c r="AS8">
+        <v>0.195372341</v>
+      </c>
+      <c r="AT8">
+        <v>0.619727849</v>
+      </c>
+      <c r="AU8">
+        <v>0.56741669100000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>0.21240880760004507</v>
+      </c>
+      <c r="C9">
+        <v>8.3132100879627011E-2</v>
+      </c>
+      <c r="D9">
+        <v>0.1160529221268705</v>
+      </c>
+      <c r="G9">
+        <v>35</v>
+      </c>
+      <c r="H9">
+        <v>0.15283386800000001</v>
+      </c>
+      <c r="I9">
+        <v>0.19498615699999999</v>
+      </c>
+      <c r="J9">
+        <v>0.11202870400000001</v>
+      </c>
+      <c r="M9">
+        <v>35</v>
+      </c>
+      <c r="N9">
+        <v>0.12116964</v>
+      </c>
+      <c r="O9">
+        <v>0.29614768600000002</v>
+      </c>
+      <c r="P9">
+        <v>0.116201965</v>
+      </c>
+      <c r="S9">
+        <v>35</v>
+      </c>
+      <c r="T9">
+        <v>0.13504717599999999</v>
+      </c>
+      <c r="U9">
+        <v>0.35631629500000001</v>
+      </c>
+      <c r="V9">
+        <v>0.12841448899999999</v>
+      </c>
+      <c r="Y9">
+        <v>35</v>
+      </c>
+      <c r="Z9">
+        <v>0.15833232799999999</v>
+      </c>
+      <c r="AA9">
+        <v>0.417304648</v>
+      </c>
+      <c r="AB9">
+        <v>0.131943372</v>
+      </c>
+      <c r="AE9">
+        <v>35</v>
+      </c>
+      <c r="AF9">
+        <v>0.152044244</v>
+      </c>
+      <c r="AG9">
+        <v>0.49393669800000001</v>
+      </c>
+      <c r="AH9">
+        <v>0.18955254899999999</v>
+      </c>
+      <c r="AL9">
+        <v>35</v>
+      </c>
+      <c r="AM9">
+        <v>0.14715890600000001</v>
+      </c>
+      <c r="AN9">
+        <v>0.63495627200000004</v>
+      </c>
+      <c r="AO9">
+        <v>0.60591082500000004</v>
+      </c>
+      <c r="AR9">
+        <v>35</v>
+      </c>
+      <c r="AS9">
+        <v>0.13041161500000001</v>
+      </c>
+      <c r="AT9">
+        <v>0.60604337699999999</v>
+      </c>
+      <c r="AU9">
+        <v>0.56692750400000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>40</v>
+      </c>
+      <c r="B10">
+        <v>5.9886610802168769E-2</v>
+      </c>
+      <c r="C10">
+        <v>8.2638374612314616E-2</v>
+      </c>
+      <c r="D10">
+        <v>0.12143541558475808</v>
+      </c>
+      <c r="G10">
+        <v>40</v>
+      </c>
+      <c r="H10">
+        <v>9.2350667999999997E-2</v>
+      </c>
+      <c r="I10">
+        <v>0.19754949999999999</v>
+      </c>
+      <c r="J10">
+        <v>0.118670527</v>
+      </c>
+      <c r="M10">
+        <v>40</v>
+      </c>
+      <c r="N10">
+        <v>0.11577794</v>
+      </c>
+      <c r="O10">
+        <v>0.28576122300000001</v>
+      </c>
+      <c r="P10">
+        <v>0.123657663</v>
+      </c>
+      <c r="S10">
+        <v>40</v>
+      </c>
+      <c r="T10">
+        <v>0.164959247</v>
+      </c>
+      <c r="U10">
+        <v>0.34705798100000002</v>
+      </c>
+      <c r="V10">
+        <v>0.13525158700000001</v>
+      </c>
+      <c r="Y10">
+        <v>40</v>
+      </c>
+      <c r="Z10">
+        <v>0.16048606100000001</v>
+      </c>
+      <c r="AA10">
+        <v>0.415369443</v>
+      </c>
+      <c r="AB10">
+        <v>0.13947631699999999</v>
+      </c>
+      <c r="AE10">
+        <v>40</v>
+      </c>
+      <c r="AF10">
+        <v>0.141631383</v>
+      </c>
+      <c r="AG10">
+        <v>0.39287102600000001</v>
+      </c>
+      <c r="AH10">
+        <v>0.22140120199999999</v>
+      </c>
+      <c r="AL10">
+        <v>40</v>
+      </c>
+      <c r="AM10">
+        <v>0.15775510100000001</v>
+      </c>
+      <c r="AN10">
+        <v>0.621473104</v>
+      </c>
+      <c r="AO10">
+        <v>0.60483277800000002</v>
+      </c>
+      <c r="AR10">
+        <v>40</v>
+      </c>
+      <c r="AS10">
+        <v>0.15091647</v>
+      </c>
+      <c r="AT10">
+        <v>0.58936261499999998</v>
+      </c>
+      <c r="AU10">
+        <v>0.56571251899999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>45</v>
+      </c>
+      <c r="B11">
+        <v>0.10198990537678812</v>
+      </c>
+      <c r="C11">
+        <v>0.11522233245006583</v>
+      </c>
+      <c r="D11">
+        <v>0.12846635250062063</v>
+      </c>
+      <c r="G11">
+        <v>45</v>
+      </c>
+      <c r="H11">
+        <v>8.3658614000000006E-2</v>
+      </c>
+      <c r="I11">
+        <v>0.199920668</v>
+      </c>
+      <c r="J11">
+        <v>0.131595405</v>
+      </c>
+      <c r="M11">
+        <v>45</v>
+      </c>
+      <c r="N11">
+        <v>0.14287544599999999</v>
+      </c>
+      <c r="O11">
+        <v>0.29692588800000003</v>
+      </c>
+      <c r="P11">
+        <v>0.134050956</v>
+      </c>
+      <c r="S11">
+        <v>45</v>
+      </c>
+      <c r="T11">
+        <v>0.111768803</v>
+      </c>
+      <c r="U11">
+        <v>0.34246352600000002</v>
+      </c>
+      <c r="V11">
+        <v>0.139147679</v>
+      </c>
+      <c r="Y11">
+        <v>45</v>
+      </c>
+      <c r="Z11">
+        <v>0.12983808099999999</v>
+      </c>
+      <c r="AA11">
+        <v>0.40827759800000002</v>
+      </c>
+      <c r="AB11">
+        <v>0.14704895100000001</v>
+      </c>
+      <c r="AE11">
+        <v>45</v>
+      </c>
+      <c r="AF11">
+        <v>0.21203239600000001</v>
+      </c>
+      <c r="AG11">
+        <v>0.31852607300000002</v>
+      </c>
+      <c r="AH11">
+        <v>0.25998965800000001</v>
+      </c>
+      <c r="AL11">
+        <v>45</v>
+      </c>
+      <c r="AM11">
+        <v>0.13382395</v>
+      </c>
+      <c r="AN11">
+        <v>0.60366289699999998</v>
+      </c>
+      <c r="AO11">
+        <v>0.60450866599999997</v>
+      </c>
+      <c r="AR11">
+        <v>45</v>
+      </c>
+      <c r="AS11">
+        <v>0.12510013</v>
+      </c>
+      <c r="AT11">
+        <v>0.57881437300000005</v>
+      </c>
+      <c r="AU11">
+        <v>0.56596915699999994</v>
+      </c>
+    </row>
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <v>4.7259464863361508E-2</v>
+      </c>
+      <c r="C12">
+        <v>8.2265765378864805E-2</v>
+      </c>
+      <c r="D12">
+        <v>0.13499768768818382</v>
+      </c>
+      <c r="G12">
+        <v>50</v>
+      </c>
+      <c r="H12">
+        <v>5.9682318999999998E-2</v>
+      </c>
+      <c r="I12">
+        <v>0.17710810900000001</v>
+      </c>
+      <c r="J12">
+        <v>0.14324272699999999</v>
+      </c>
+      <c r="M12">
+        <v>50</v>
+      </c>
+      <c r="N12">
+        <v>7.7781384999999995E-2</v>
+      </c>
+      <c r="O12">
+        <v>0.30026494100000001</v>
+      </c>
+      <c r="P12">
+        <v>0.14312531100000001</v>
+      </c>
+      <c r="S12">
+        <v>50</v>
+      </c>
+      <c r="T12">
+        <v>9.8400080000000001E-2</v>
+      </c>
+      <c r="U12">
+        <v>0.33571836100000002</v>
+      </c>
+      <c r="V12">
+        <v>0.149502937</v>
+      </c>
+      <c r="Y12">
+        <v>50</v>
+      </c>
+      <c r="Z12">
+        <v>0.115831038</v>
+      </c>
+      <c r="AA12">
+        <v>0.401647808</v>
+      </c>
+      <c r="AB12">
+        <v>0.152172115</v>
+      </c>
+      <c r="AE12">
+        <v>50</v>
+      </c>
+      <c r="AF12">
+        <v>0.12526781100000001</v>
+      </c>
+      <c r="AG12">
+        <v>0.25993512000000002</v>
+      </c>
+      <c r="AH12">
+        <v>0.28433275800000002</v>
+      </c>
+      <c r="AL12">
+        <v>50</v>
+      </c>
+      <c r="AM12">
+        <v>0.13740297200000001</v>
+      </c>
+      <c r="AN12">
+        <v>0.59897141499999995</v>
+      </c>
+      <c r="AO12">
+        <v>0.60466670499999997</v>
+      </c>
+      <c r="AR12">
+        <v>50</v>
+      </c>
+      <c r="AS12">
+        <v>0.131646547</v>
+      </c>
+      <c r="AT12">
+        <v>0.573587548</v>
+      </c>
+      <c r="AU12">
+        <v>0.56607788199999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>55</v>
+      </c>
+      <c r="B13">
+        <v>3.9854955597792625E-2</v>
+      </c>
+      <c r="C13">
+        <v>5.8534405235625336E-2</v>
+      </c>
+      <c r="D13">
+        <v>0.14176773091325995</v>
+      </c>
+      <c r="G13">
+        <v>55</v>
+      </c>
+      <c r="H13">
+        <v>5.5657303999999998E-2</v>
+      </c>
+      <c r="I13">
+        <v>0.15945099600000001</v>
+      </c>
+      <c r="J13">
+        <v>0.15300440100000001</v>
+      </c>
+      <c r="M13">
+        <v>55</v>
+      </c>
+      <c r="N13">
+        <v>0.15135605399999999</v>
+      </c>
+      <c r="O13">
+        <v>0.28575205599999998</v>
+      </c>
+      <c r="P13">
+        <v>0.15103615200000001</v>
+      </c>
+      <c r="S13">
+        <v>55</v>
+      </c>
+      <c r="T13">
+        <v>8.7530646000000004E-2</v>
+      </c>
+      <c r="U13">
+        <v>0.33064940999999998</v>
+      </c>
+      <c r="V13">
+        <v>0.158579362</v>
+      </c>
+      <c r="Y13">
+        <v>55</v>
+      </c>
+      <c r="Z13">
+        <v>0.10166409</v>
+      </c>
+      <c r="AA13">
+        <v>0.39938282000000003</v>
+      </c>
+      <c r="AB13">
+        <v>0.16014302499999999</v>
+      </c>
+      <c r="AE13">
+        <v>55</v>
+      </c>
+      <c r="AF13">
+        <v>0.111657335</v>
+      </c>
+      <c r="AG13">
+        <v>0.23447789299999999</v>
+      </c>
+      <c r="AH13">
+        <v>0.300665609</v>
+      </c>
+      <c r="AL13">
+        <v>55</v>
+      </c>
+      <c r="AM13">
+        <v>0.106586004</v>
+      </c>
+      <c r="AN13">
+        <v>0.59497106099999997</v>
+      </c>
+      <c r="AO13">
+        <v>0.60469545199999997</v>
+      </c>
+      <c r="AR13">
+        <v>55</v>
+      </c>
+      <c r="AS13">
+        <v>0.12945211400000001</v>
+      </c>
+      <c r="AT13">
+        <v>0.560831517</v>
+      </c>
+      <c r="AU13">
+        <v>0.56591628299999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>60</v>
+      </c>
+      <c r="B14">
+        <v>6.0256315366423022E-2</v>
+      </c>
+      <c r="C14">
+        <v>6.7018756906018939E-2</v>
+      </c>
+      <c r="D14">
+        <v>0.14800412540388047</v>
+      </c>
+      <c r="G14">
+        <v>60</v>
+      </c>
+      <c r="H14">
+        <v>5.1335540999999998E-2</v>
+      </c>
+      <c r="I14">
+        <v>0.15000920600000001</v>
+      </c>
+      <c r="J14">
+        <v>0.15980971699999999</v>
+      </c>
+      <c r="M14">
+        <v>60</v>
+      </c>
+      <c r="N14">
+        <v>0.12536702599999999</v>
+      </c>
+      <c r="O14">
+        <v>0.26374796900000003</v>
+      </c>
+      <c r="P14">
+        <v>0.15689365699999999</v>
+      </c>
+      <c r="S14">
+        <v>60</v>
+      </c>
+      <c r="T14">
+        <v>8.4023404999999995E-2</v>
+      </c>
+      <c r="U14">
+        <v>0.33185492900000002</v>
+      </c>
+      <c r="V14">
+        <v>0.165325364</v>
+      </c>
+      <c r="Y14">
+        <v>60</v>
+      </c>
+      <c r="Z14">
+        <v>9.8101517999999999E-2</v>
+      </c>
+      <c r="AA14">
+        <v>0.396616315</v>
+      </c>
+      <c r="AB14">
+        <v>0.16659590899999999</v>
+      </c>
+      <c r="AE14">
+        <v>60</v>
+      </c>
+      <c r="AF14">
+        <v>9.4060232999999993E-2</v>
+      </c>
+      <c r="AG14">
+        <v>0.228822055</v>
+      </c>
+      <c r="AH14">
+        <v>0.320151772</v>
+      </c>
+      <c r="AL14">
+        <v>60</v>
+      </c>
+      <c r="AM14">
+        <v>8.6785669999999995E-2</v>
+      </c>
+      <c r="AN14">
+        <v>0.560488129</v>
+      </c>
+      <c r="AO14">
+        <v>0.58872023699999998</v>
+      </c>
+      <c r="AR14">
+        <v>60</v>
+      </c>
+      <c r="AS14">
+        <v>0.106929602</v>
+      </c>
+      <c r="AT14">
+        <v>0.55373905499999998</v>
+      </c>
+      <c r="AU14">
+        <v>0.56598253899999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>65</v>
+      </c>
+      <c r="B15">
+        <v>2.6111122854748897E-2</v>
+      </c>
+      <c r="C15">
+        <v>4.0664965275924531E-2</v>
+      </c>
+      <c r="D15">
+        <v>0.15393801797023135</v>
+      </c>
+      <c r="G15">
+        <v>65</v>
+      </c>
+      <c r="H15">
+        <v>4.0274592999999997E-2</v>
+      </c>
+      <c r="I15">
+        <v>0.145698366</v>
+      </c>
+      <c r="J15">
+        <v>0.16649161000000001</v>
+      </c>
+      <c r="M15">
+        <v>65</v>
+      </c>
+      <c r="N15">
+        <v>7.3607425000000004E-2</v>
+      </c>
+      <c r="O15">
+        <v>0.25274609300000001</v>
+      </c>
+      <c r="P15">
+        <v>0.16363217499999999</v>
+      </c>
+      <c r="S15">
+        <v>65</v>
+      </c>
+      <c r="T15">
+        <v>0.10962912399999999</v>
+      </c>
+      <c r="U15">
+        <v>0.32566711300000001</v>
+      </c>
+      <c r="V15">
+        <v>0.171305236</v>
+      </c>
+      <c r="Y15">
+        <v>65</v>
+      </c>
+      <c r="Z15">
+        <v>9.4491338999999994E-2</v>
+      </c>
+      <c r="AA15">
+        <v>0.316827046</v>
+      </c>
+      <c r="AB15">
+        <v>0.199055712</v>
+      </c>
+      <c r="AE15">
+        <v>65</v>
+      </c>
+      <c r="AF15">
+        <v>9.3326419999999993E-2</v>
+      </c>
+      <c r="AG15">
+        <v>0.19865349900000001</v>
+      </c>
+      <c r="AH15">
+        <v>0.33684429900000001</v>
+      </c>
+      <c r="AL15">
+        <v>65</v>
+      </c>
+      <c r="AM15">
+        <v>9.8436767999999994E-2</v>
+      </c>
+      <c r="AN15">
+        <v>0.48778884700000003</v>
+      </c>
+      <c r="AO15">
+        <v>0.55263984899999996</v>
+      </c>
+      <c r="AR15">
+        <v>65</v>
+      </c>
+      <c r="AS15">
+        <v>0.11482676999999999</v>
+      </c>
+      <c r="AT15">
+        <v>0.55185037199999998</v>
+      </c>
+      <c r="AU15">
+        <v>0.56613070300000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>70</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0.1594731806890049</v>
+      </c>
+      <c r="G16">
+        <v>70</v>
+      </c>
+      <c r="H16">
+        <v>4.3706910000000002E-2</v>
+      </c>
+      <c r="I16">
+        <v>0.14336397200000001</v>
+      </c>
+      <c r="J16">
+        <v>0.17166374100000001</v>
+      </c>
+      <c r="M16">
+        <v>70</v>
+      </c>
+      <c r="N16">
+        <v>7.4518695999999995E-2</v>
+      </c>
+      <c r="O16">
+        <v>0.25008530600000001</v>
+      </c>
+      <c r="P16">
+        <v>0.168660959</v>
+      </c>
+      <c r="S16">
+        <v>70</v>
+      </c>
+      <c r="T16">
+        <v>0.104756764</v>
+      </c>
+      <c r="U16">
+        <v>0.32843063500000003</v>
+      </c>
+      <c r="V16">
+        <v>0.17381618500000001</v>
+      </c>
+      <c r="Y16">
+        <v>70</v>
+      </c>
+      <c r="Z16">
+        <v>9.5630207999999994E-2</v>
+      </c>
+      <c r="AA16">
+        <v>0.26495676699999998</v>
+      </c>
+      <c r="AB16">
+        <v>0.223298674</v>
+      </c>
+      <c r="AE16">
+        <v>70</v>
+      </c>
+      <c r="AF16">
+        <v>0.11628860100000001</v>
+      </c>
+      <c r="AG16">
+        <v>0.18309719999999999</v>
+      </c>
+      <c r="AH16">
+        <v>0.35717711200000002</v>
+      </c>
+      <c r="AL16">
+        <v>70</v>
+      </c>
+      <c r="AM16">
+        <v>0.115917296</v>
+      </c>
+      <c r="AN16">
+        <v>0.43231907800000002</v>
+      </c>
+      <c r="AO16">
+        <v>0.521307089</v>
+      </c>
+      <c r="AR16">
+        <v>70</v>
+      </c>
+      <c r="AS16">
+        <v>0.138076111</v>
+      </c>
+      <c r="AT16">
+        <v>0.52180240700000002</v>
+      </c>
+      <c r="AU16">
+        <v>0.55513288299999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>153</v>
+      </c>
+      <c r="C19" t="s">
+        <v>154</v>
+      </c>
+      <c r="D19" t="s">
+        <v>155</v>
+      </c>
+      <c r="E19" t="s">
+        <v>156</v>
+      </c>
+      <c r="F19" t="s">
+        <v>157</v>
+      </c>
+      <c r="G19" t="s">
+        <v>158</v>
+      </c>
+      <c r="H19" t="s">
+        <v>159</v>
+      </c>
+      <c r="I19" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>0.2108511535458267</v>
+      </c>
+      <c r="C20">
+        <v>0.190878978</v>
+      </c>
+      <c r="D20">
+        <v>0.179495399</v>
+      </c>
+      <c r="E20">
+        <v>0.17321540099999999</v>
+      </c>
+      <c r="F20">
+        <v>0.151891045</v>
+      </c>
+      <c r="G20">
+        <v>0.17253289599999999</v>
+      </c>
+      <c r="H20">
+        <v>0.60561447899999998</v>
+      </c>
+      <c r="I20">
+        <v>0.57044078099999995</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>10</v>
+      </c>
+      <c r="B21">
+        <v>0.21085115354582662</v>
+      </c>
+      <c r="C21">
+        <v>0.190878978</v>
+      </c>
+      <c r="D21">
+        <v>0.179495399</v>
+      </c>
+      <c r="E21">
+        <v>0.17321540099999999</v>
+      </c>
+      <c r="F21">
+        <v>0.15819113400000001</v>
+      </c>
+      <c r="G21">
+        <v>0.17253289599999999</v>
+      </c>
+      <c r="H21">
+        <v>0.606660541</v>
+      </c>
+      <c r="I21">
+        <v>0.56909805000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>15</v>
+      </c>
+      <c r="B22">
+        <v>0.21085115354582673</v>
+      </c>
+      <c r="C22">
+        <v>0.190878978</v>
+      </c>
+      <c r="D22">
+        <v>0.179495399</v>
+      </c>
+      <c r="E22">
+        <v>0.17321540099999999</v>
+      </c>
+      <c r="F22">
+        <v>0.16161914199999999</v>
+      </c>
+      <c r="G22">
+        <v>0.17253289599999999</v>
+      </c>
+      <c r="H22">
+        <v>0.60649472999999998</v>
+      </c>
+      <c r="I22">
+        <v>0.56874962299999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>0.16966621725300246</v>
+      </c>
+      <c r="C23">
+        <v>0.15486550099999999</v>
+      </c>
+      <c r="D23">
+        <v>0.14511374599999999</v>
+      </c>
+      <c r="E23">
+        <v>0.14105674900000001</v>
+      </c>
+      <c r="F23">
+        <v>0.14404299200000001</v>
+      </c>
+      <c r="G23">
+        <v>0.16570743099999999</v>
+      </c>
+      <c r="H23">
+        <v>0.60630627199999998</v>
+      </c>
+      <c r="I23">
+        <v>0.56795775599999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>25</v>
+      </c>
+      <c r="B24">
+        <v>0.13859000277215855</v>
+      </c>
+      <c r="C24">
+        <v>0.13111799399999999</v>
+      </c>
+      <c r="D24">
+        <v>0.12653077700000001</v>
+      </c>
+      <c r="E24">
+        <v>0.12363901400000001</v>
+      </c>
+      <c r="F24">
+        <v>0.13298987600000001</v>
+      </c>
+      <c r="G24">
+        <v>0.171088501</v>
+      </c>
+      <c r="H24">
+        <v>0.60601994100000001</v>
+      </c>
+      <c r="I24">
+        <v>0.56783326300000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>30</v>
+      </c>
+      <c r="B25">
+        <v>0.12220452672241615</v>
+      </c>
+      <c r="C25">
+        <v>0.118521707</v>
+      </c>
+      <c r="D25">
+        <v>0.11970107100000001</v>
+      </c>
+      <c r="E25">
+        <v>0.12211119500000001</v>
+      </c>
+      <c r="F25">
+        <v>0.12891243999999999</v>
+      </c>
+      <c r="G25">
+        <v>0.177861084</v>
+      </c>
+      <c r="H25">
+        <v>0.60595386299999998</v>
+      </c>
+      <c r="I25">
+        <v>0.56741669100000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>35</v>
+      </c>
+      <c r="B26">
+        <v>0.1160529221268705</v>
+      </c>
+      <c r="C26">
+        <v>0.11202870400000001</v>
+      </c>
+      <c r="D26">
+        <v>0.116201965</v>
+      </c>
+      <c r="E26">
+        <v>0.12841448899999999</v>
+      </c>
+      <c r="F26">
+        <v>0.131943372</v>
+      </c>
+      <c r="G26">
+        <v>0.18955254899999999</v>
+      </c>
+      <c r="H26">
+        <v>0.60591082500000004</v>
+      </c>
+      <c r="I26">
+        <v>0.56692750400000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>40</v>
+      </c>
+      <c r="B27">
+        <v>0.12143541558475808</v>
+      </c>
+      <c r="C27">
+        <v>0.118670527</v>
+      </c>
+      <c r="D27">
+        <v>0.123657663</v>
+      </c>
+      <c r="E27">
+        <v>0.13525158700000001</v>
+      </c>
+      <c r="F27">
+        <v>0.13947631699999999</v>
+      </c>
+      <c r="G27">
+        <v>0.22140120199999999</v>
+      </c>
+      <c r="H27">
+        <v>0.60483277800000002</v>
+      </c>
+      <c r="I27">
+        <v>0.56571251899999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>45</v>
+      </c>
+      <c r="B28">
+        <v>0.12846635250062063</v>
+      </c>
+      <c r="C28">
+        <v>0.131595405</v>
+      </c>
+      <c r="D28">
+        <v>0.134050956</v>
+      </c>
+      <c r="E28">
+        <v>0.139147679</v>
+      </c>
+      <c r="F28">
+        <v>0.14704895100000001</v>
+      </c>
+      <c r="G28">
+        <v>0.25998965800000001</v>
+      </c>
+      <c r="H28">
+        <v>0.60450866599999997</v>
+      </c>
+      <c r="I28">
+        <v>0.56596915699999994</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>50</v>
+      </c>
+      <c r="B29">
+        <v>0.13499768768818382</v>
+      </c>
+      <c r="C29">
+        <v>0.14324272699999999</v>
+      </c>
+      <c r="D29">
+        <v>0.14312531100000001</v>
+      </c>
+      <c r="E29">
+        <v>0.149502937</v>
+      </c>
+      <c r="F29">
+        <v>0.152172115</v>
+      </c>
+      <c r="G29">
+        <v>0.28433275800000002</v>
+      </c>
+      <c r="H29">
+        <v>0.60466670499999997</v>
+      </c>
+      <c r="I29">
+        <v>0.56607788199999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>55</v>
+      </c>
+      <c r="B30">
+        <v>0.14176773091325995</v>
+      </c>
+      <c r="C30">
+        <v>0.15300440100000001</v>
+      </c>
+      <c r="D30">
+        <v>0.15103615200000001</v>
+      </c>
+      <c r="E30">
+        <v>0.158579362</v>
+      </c>
+      <c r="F30">
+        <v>0.16014302499999999</v>
+      </c>
+      <c r="G30">
+        <v>0.300665609</v>
+      </c>
+      <c r="H30">
+        <v>0.60469545199999997</v>
+      </c>
+      <c r="I30">
+        <v>0.56591628299999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>60</v>
+      </c>
+      <c r="B31">
+        <v>0.14800412540388047</v>
+      </c>
+      <c r="C31">
+        <v>0.15980971699999999</v>
+      </c>
+      <c r="D31">
+        <v>0.15689365699999999</v>
+      </c>
+      <c r="E31">
+        <v>0.165325364</v>
+      </c>
+      <c r="F31">
+        <v>0.16659590899999999</v>
+      </c>
+      <c r="G31">
+        <v>0.320151772</v>
+      </c>
+      <c r="H31">
+        <v>0.58872023699999998</v>
+      </c>
+      <c r="I31">
+        <v>0.56598253899999995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>65</v>
+      </c>
+      <c r="B32">
+        <v>0.15393801797023135</v>
+      </c>
+      <c r="C32">
+        <v>0.16649161000000001</v>
+      </c>
+      <c r="D32">
+        <v>0.16363217499999999</v>
+      </c>
+      <c r="E32">
+        <v>0.171305236</v>
+      </c>
+      <c r="F32">
+        <v>0.199055712</v>
+      </c>
+      <c r="G32">
+        <v>0.33684429900000001</v>
+      </c>
+      <c r="H32">
+        <v>0.55263984899999996</v>
+      </c>
+      <c r="I32">
+        <v>0.56613070300000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>70</v>
+      </c>
+      <c r="B33">
+        <v>0.1594731806890049</v>
+      </c>
+      <c r="C33">
+        <v>0.17166374100000001</v>
+      </c>
+      <c r="D33">
+        <v>0.168660959</v>
+      </c>
+      <c r="E33">
+        <v>0.17381618500000001</v>
+      </c>
+      <c r="F33">
+        <v>0.223298674</v>
+      </c>
+      <c r="G33">
+        <v>0.35717711200000002</v>
+      </c>
+      <c r="H33">
+        <v>0.521307089</v>
+      </c>
+      <c r="I33">
+        <v>0.55513288299999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>